<commit_message>
fix urban & farmland area
</commit_message>
<xml_diff>
--- a/Medieval Info.xlsx
+++ b/Medieval Info.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="163">
   <si>
     <t>Link</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>Urban area per person (m²)</t>
+  </si>
+  <si>
+    <t>Urban area per person (ha=100m*100m)</t>
   </si>
   <si>
     <t>Urban construction height</t>
@@ -990,11 +993,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="683644857"/>
-        <c:axId val="224973707"/>
+        <c:axId val="532613063"/>
+        <c:axId val="319222459"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="683644857"/>
+        <c:axId val="532613063"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1046,10 +1049,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224973707"/>
+        <c:crossAx val="319222459"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="224973707"/>
+        <c:axId val="319222459"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1124,7 +1127,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="683644857"/>
+        <c:crossAx val="532613063"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1216,11 +1219,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1971967435"/>
-        <c:axId val="1989495374"/>
+        <c:axId val="422504406"/>
+        <c:axId val="567235271"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1971967435"/>
+        <c:axId val="422504406"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1272,10 +1275,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1989495374"/>
+        <c:crossAx val="567235271"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1989495374"/>
+        <c:axId val="567235271"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1350,7 +1353,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1971967435"/>
+        <c:crossAx val="422504406"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1506,11 +1509,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="825611771"/>
-        <c:axId val="1036434370"/>
+        <c:axId val="157024430"/>
+        <c:axId val="1984777209"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="825611771"/>
+        <c:axId val="157024430"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1562,10 +1565,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1036434370"/>
+        <c:crossAx val="1984777209"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1036434370"/>
+        <c:axId val="1984777209"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1640,7 +1643,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="825611771"/>
+        <c:crossAx val="157024430"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1765,11 +1768,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1042722625"/>
-        <c:axId val="1879532893"/>
+        <c:axId val="1344402790"/>
+        <c:axId val="348381166"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1042722625"/>
+        <c:axId val="1344402790"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1821,10 +1824,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1879532893"/>
+        <c:crossAx val="348381166"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1879532893"/>
+        <c:axId val="348381166"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1899,7 +1902,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1042722625"/>
+        <c:crossAx val="1344402790"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2024,11 +2027,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="373260128"/>
-        <c:axId val="1289869689"/>
+        <c:axId val="2130729286"/>
+        <c:axId val="1265249093"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="373260128"/>
+        <c:axId val="2130729286"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2080,10 +2083,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1289869689"/>
+        <c:crossAx val="1265249093"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1289869689"/>
+        <c:axId val="1265249093"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2158,7 +2161,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373260128"/>
+        <c:crossAx val="2130729286"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2920,54 +2923,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B2" s="4">
         <v>80.0</v>
@@ -3011,7 +3014,7 @@
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B3" s="4">
         <v>5.0</v>
@@ -3037,7 +3040,7 @@
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B4" s="4">
         <v>5.0</v>
@@ -3075,7 +3078,7 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B5" s="4">
         <v>5.0</v>
@@ -3083,7 +3086,7 @@
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B6" s="4">
         <v>5.0</v>
@@ -3091,22 +3094,22 @@
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B10" s="12">
         <f>SUM(B2:B9)</f>
@@ -3132,14 +3135,14 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -3158,21 +3161,21 @@
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
@@ -3183,21 +3186,21 @@
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
@@ -3208,21 +3211,21 @@
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
@@ -3233,39 +3236,39 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
@@ -3280,7 +3283,7 @@
         <v>34</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D6" s="4">
         <f>9057</f>
@@ -3407,7 +3410,7 @@
     </row>
     <row r="9">
       <c r="C9" s="10" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" ref="D9:G9" si="1">SUM(D11:D18)</f>
@@ -3452,7 +3455,7 @@
     </row>
     <row r="10">
       <c r="C10" s="10" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" ref="D10:G10" si="3">ROUNDUP(AVERAGE(D7,D8))-D9</f>
@@ -3497,13 +3500,13 @@
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D11" s="4">
         <v>2.0</v>
@@ -3539,7 +3542,7 @@
     </row>
     <row r="12">
       <c r="C12" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D12" s="4">
         <v>2.0</v>
@@ -3563,7 +3566,7 @@
     </row>
     <row r="13">
       <c r="C13" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E13" s="4">
         <v>3.0</v>
@@ -3583,7 +3586,7 @@
     </row>
     <row r="14">
       <c r="C14" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D14" s="4">
         <v>1.0</v>
@@ -3613,7 +3616,7 @@
     </row>
     <row r="15">
       <c r="C15" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D15" s="4">
         <v>2.0</v>
@@ -3646,7 +3649,7 @@
     </row>
     <row r="16">
       <c r="C16" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D16" s="4">
         <v>1.0</v>
@@ -3660,7 +3663,7 @@
     </row>
     <row r="17">
       <c r="C17" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D17" s="4">
         <v>1.0</v>
@@ -3671,7 +3674,7 @@
     </row>
     <row r="18">
       <c r="C18" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D18" s="4">
         <v>1.0</v>
@@ -3698,13 +3701,13 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D19" s="12">
         <f>SUMPRODUCT(D11:D18,Citizens!$B$3:$B$10)</f>
@@ -3745,7 +3748,7 @@
     </row>
     <row r="20">
       <c r="C20" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D20" s="12">
         <f>SUMPRODUCT(D11:D18,Citizens!$C$3:$C$10)</f>
@@ -3786,13 +3789,13 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D21" s="12">
         <f>SUMPRODUCT(D11:D18,Citizens!$D$3:$D$10)</f>
@@ -3833,7 +3836,7 @@
     </row>
     <row r="22">
       <c r="C22" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D22" s="12">
         <f>SUMPRODUCT(D11:D18,Citizens!$E$3:$E$10)</f>
@@ -3874,13 +3877,13 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D23" s="12">
         <f t="shared" ref="D23:G23" si="5">D21+D19</f>
@@ -3921,7 +3924,7 @@
     </row>
     <row r="24">
       <c r="C24" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D24" s="12">
         <f t="shared" ref="D24:G24" si="7">D22+D20</f>
@@ -3962,13 +3965,13 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D25" s="12" t="b">
         <f t="shared" ref="D25:G25" si="10">D12&gt;0</f>
@@ -4009,7 +4012,7 @@
     </row>
     <row r="26">
       <c r="C26" s="10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D26" s="12" t="b">
         <f t="shared" ref="D26:G26" si="12">D18&gt;0</f>
@@ -4050,7 +4053,7 @@
     </row>
     <row r="27">
       <c r="C27" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D27" s="12" t="b">
         <f t="shared" ref="D27:G27" si="14">D16&gt;0</f>
@@ -4091,7 +4094,7 @@
     </row>
     <row r="28">
       <c r="C28" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D28" s="12" t="b">
         <f t="shared" ref="D28:G28" si="16">D17&gt;0</f>
@@ -4132,7 +4135,7 @@
     </row>
     <row r="29">
       <c r="C29" s="10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D29" s="12" t="b">
         <f t="shared" ref="D29:G29" si="19">D14&gt;0</f>
@@ -4173,7 +4176,7 @@
     </row>
     <row r="30">
       <c r="C30" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D30" s="12" t="b">
         <f t="shared" ref="D30:G30" si="21">D15&gt;0</f>
@@ -4214,29 +4217,29 @@
     </row>
     <row r="31">
       <c r="A31" s="17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D31" s="15">
         <f>D$9*'Land Use'!$D3</f>
-        <v>1500</v>
+        <v>3.75</v>
       </c>
       <c r="E31" s="15">
         <f>E$9*'Land Use'!$D3</f>
-        <v>1350</v>
+        <v>3.375</v>
       </c>
       <c r="F31" s="15">
         <f>F$9*'Land Use'!$D3</f>
-        <v>900</v>
+        <v>2.25</v>
       </c>
       <c r="G31" s="15">
         <f>G$9*'Land Use'!$D3</f>
-        <v>600</v>
+        <v>1.5</v>
       </c>
       <c r="H31" s="15">
         <f>H$9*'Land Use'!$D3</f>
@@ -4244,7 +4247,7 @@
       </c>
       <c r="I31" s="15">
         <f>I$9*'Land Use'!$D3</f>
-        <v>5850</v>
+        <v>14.625</v>
       </c>
       <c r="J31" s="15"/>
       <c r="K31" s="15"/>
@@ -4252,40 +4255,40 @@
       <c r="M31" s="15"/>
       <c r="N31" s="15">
         <f>N$9*'Land Use'!$D3</f>
-        <v>900</v>
+        <v>2.25</v>
       </c>
       <c r="O31" s="15">
         <f>O$9*'Land Use'!$D3</f>
-        <v>1200</v>
+        <v>3</v>
       </c>
       <c r="P31" s="15">
         <f>P$9*'Land Use'!$D3</f>
-        <v>2400</v>
+        <v>6</v>
       </c>
       <c r="Q31" s="15">
         <f>Q$9*'Land Use'!$D3</f>
-        <v>900</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="32">
       <c r="C32" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D32" s="15">
         <f>D$9*'Land Use'!$D4</f>
-        <v>3333.333333</v>
+        <v>50</v>
       </c>
       <c r="E32" s="15">
         <f>E$9*'Land Use'!$D4</f>
-        <v>3000</v>
+        <v>45</v>
       </c>
       <c r="F32" s="15">
         <f>F$9*'Land Use'!$D4</f>
-        <v>2000</v>
+        <v>30</v>
       </c>
       <c r="G32" s="15">
         <f>G$9*'Land Use'!$D4</f>
-        <v>1333.333333</v>
+        <v>20</v>
       </c>
       <c r="H32" s="15">
         <f>H$9*'Land Use'!$D4</f>
@@ -4293,7 +4296,7 @@
       </c>
       <c r="I32" s="15">
         <f>I$9*'Land Use'!$D4</f>
-        <v>13000</v>
+        <v>195</v>
       </c>
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
@@ -4301,45 +4304,45 @@
       <c r="M32" s="15"/>
       <c r="N32" s="15">
         <f>N$9*'Land Use'!$D4</f>
-        <v>2000</v>
+        <v>30</v>
       </c>
       <c r="O32" s="15">
         <f>O$9*'Land Use'!$D4</f>
-        <v>2666.666667</v>
+        <v>40</v>
       </c>
       <c r="P32" s="15">
         <f>P$9*'Land Use'!$D4</f>
-        <v>5333.333333</v>
+        <v>80</v>
       </c>
       <c r="Q32" s="15">
         <f>Q$9*'Land Use'!$D4</f>
-        <v>2000</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33">
       <c r="C33" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D33" s="15">
         <f t="shared" ref="D33:G33" si="24">D31*100^2/25^2</f>
-        <v>24000</v>
+        <v>60</v>
       </c>
       <c r="E33" s="15">
         <f t="shared" si="24"/>
-        <v>21600</v>
+        <v>54</v>
       </c>
       <c r="F33" s="15">
         <f t="shared" si="24"/>
-        <v>14400</v>
+        <v>36</v>
       </c>
       <c r="G33" s="15">
         <f t="shared" si="24"/>
-        <v>9600</v>
+        <v>24</v>
       </c>
       <c r="H33" s="15"/>
       <c r="I33" s="15">
         <f t="shared" ref="I33:I34" si="27">I31*100^2/25^2</f>
-        <v>93600</v>
+        <v>234</v>
       </c>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
@@ -4347,45 +4350,45 @@
       <c r="M33" s="15"/>
       <c r="N33" s="15">
         <f t="shared" ref="N33:Q33" si="25">N31*100^2/25^2</f>
-        <v>14400</v>
+        <v>36</v>
       </c>
       <c r="O33" s="15">
         <f t="shared" si="25"/>
-        <v>19200</v>
+        <v>48</v>
       </c>
       <c r="P33" s="15">
         <f t="shared" si="25"/>
-        <v>38400</v>
+        <v>96</v>
       </c>
       <c r="Q33" s="15">
         <f t="shared" si="25"/>
-        <v>14400</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34">
       <c r="C34" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D34" s="15">
         <f t="shared" ref="D34:G34" si="26">D32*100^2/25^2</f>
-        <v>53333.33333</v>
+        <v>800</v>
       </c>
       <c r="E34" s="15">
         <f t="shared" si="26"/>
-        <v>48000</v>
+        <v>720</v>
       </c>
       <c r="F34" s="15">
         <f t="shared" si="26"/>
-        <v>32000</v>
+        <v>480</v>
       </c>
       <c r="G34" s="15">
         <f t="shared" si="26"/>
-        <v>21333.33333</v>
+        <v>320</v>
       </c>
       <c r="H34" s="15"/>
       <c r="I34" s="15">
         <f t="shared" si="27"/>
-        <v>208000</v>
+        <v>3120</v>
       </c>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
@@ -4393,48 +4396,48 @@
       <c r="M34" s="15"/>
       <c r="N34" s="15">
         <f t="shared" ref="N34:Q34" si="28">N32*100^2/25^2</f>
-        <v>32000</v>
+        <v>480</v>
       </c>
       <c r="O34" s="15">
         <f t="shared" si="28"/>
-        <v>42666.66667</v>
+        <v>640</v>
       </c>
       <c r="P34" s="15">
         <f t="shared" si="28"/>
-        <v>85333.33333</v>
+        <v>1280</v>
       </c>
       <c r="Q34" s="15">
         <f t="shared" si="28"/>
-        <v>32000</v>
+        <v>480</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" s="18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D35" s="15">
         <f t="shared" ref="D35:G35" si="29">ROUNDUP(SQRT(D31))</f>
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="E35" s="15">
         <f t="shared" si="29"/>
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="F35" s="15">
         <f t="shared" si="29"/>
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="G35" s="15">
         <f t="shared" si="29"/>
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="H35" s="15"/>
       <c r="I35" s="15">
         <f t="shared" ref="I35:I38" si="32">ROUNDUP(SQRT(I31))</f>
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
@@ -4442,45 +4445,45 @@
       <c r="M35" s="15"/>
       <c r="N35" s="15">
         <f t="shared" ref="N35:Q35" si="30">ROUNDUP(SQRT(N31))</f>
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="O35" s="15">
         <f t="shared" si="30"/>
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="P35" s="15">
         <f t="shared" si="30"/>
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="Q35" s="15">
         <f t="shared" si="30"/>
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
       <c r="C36" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D36" s="15">
         <f t="shared" ref="D36:G36" si="31">ROUNDUP(SQRT(D32))</f>
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="E36" s="15">
         <f t="shared" si="31"/>
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="F36" s="15">
         <f t="shared" si="31"/>
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="G36" s="15">
         <f t="shared" si="31"/>
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="H36" s="15"/>
       <c r="I36" s="15">
         <f t="shared" si="32"/>
-        <v>115</v>
+        <v>14</v>
       </c>
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
@@ -4488,45 +4491,45 @@
       <c r="M36" s="15"/>
       <c r="N36" s="15">
         <f t="shared" ref="N36:Q36" si="33">ROUNDUP(SQRT(N32))</f>
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="O36" s="15">
         <f t="shared" si="33"/>
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="P36" s="15">
         <f t="shared" si="33"/>
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="Q36" s="15">
         <f t="shared" si="33"/>
-        <v>45</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37">
       <c r="C37" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D37" s="15">
         <f t="shared" ref="D37:G37" si="34">ROUNDUP(SQRT(D33))</f>
-        <v>155</v>
+        <v>8</v>
       </c>
       <c r="E37" s="15">
         <f t="shared" si="34"/>
-        <v>147</v>
+        <v>8</v>
       </c>
       <c r="F37" s="15">
         <f t="shared" si="34"/>
-        <v>120</v>
+        <v>6</v>
       </c>
       <c r="G37" s="15">
         <f t="shared" si="34"/>
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="H37" s="15"/>
       <c r="I37" s="15">
         <f t="shared" si="32"/>
-        <v>306</v>
+        <v>16</v>
       </c>
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>
@@ -4534,45 +4537,45 @@
       <c r="M37" s="15"/>
       <c r="N37" s="15">
         <f t="shared" ref="N37:Q37" si="35">ROUNDUP(SQRT(N33))</f>
-        <v>120</v>
+        <v>6</v>
       </c>
       <c r="O37" s="15">
         <f t="shared" si="35"/>
-        <v>139</v>
+        <v>7</v>
       </c>
       <c r="P37" s="15">
         <f t="shared" si="35"/>
-        <v>196</v>
+        <v>10</v>
       </c>
       <c r="Q37" s="15">
         <f t="shared" si="35"/>
-        <v>120</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38">
       <c r="C38" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D38" s="15">
         <f t="shared" ref="D38:G38" si="36">ROUNDUP(SQRT(D34))</f>
-        <v>231</v>
+        <v>29</v>
       </c>
       <c r="E38" s="15">
         <f t="shared" si="36"/>
-        <v>220</v>
+        <v>27</v>
       </c>
       <c r="F38" s="15">
         <f t="shared" si="36"/>
-        <v>179</v>
+        <v>22</v>
       </c>
       <c r="G38" s="15">
         <f t="shared" si="36"/>
-        <v>147</v>
+        <v>18</v>
       </c>
       <c r="H38" s="15"/>
       <c r="I38" s="15">
         <f t="shared" si="32"/>
-        <v>457</v>
+        <v>56</v>
       </c>
       <c r="J38" s="15"/>
       <c r="K38" s="15"/>
@@ -4580,30 +4583,30 @@
       <c r="M38" s="15"/>
       <c r="N38" s="15">
         <f t="shared" ref="N38:Q38" si="37">ROUNDUP(SQRT(N34))</f>
-        <v>179</v>
+        <v>22</v>
       </c>
       <c r="O38" s="15">
         <f t="shared" si="37"/>
-        <v>207</v>
+        <v>26</v>
       </c>
       <c r="P38" s="15">
         <f t="shared" si="37"/>
-        <v>293</v>
+        <v>36</v>
       </c>
       <c r="Q38" s="15">
         <f t="shared" si="37"/>
-        <v>179</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D39" s="15">
         <f>D$11*'Land Use'!$C3</f>
@@ -4652,7 +4655,7 @@
     </row>
     <row r="40">
       <c r="C40" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D40" s="15">
         <f>D$11*'Land Use'!$C4</f>
@@ -4701,7 +4704,7 @@
     </row>
     <row r="41">
       <c r="C41" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D41" s="15">
         <f t="shared" ref="D41:G41" si="38">D39*100^2/25^2</f>
@@ -4747,7 +4750,7 @@
     </row>
     <row r="42">
       <c r="C42" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D42" s="15">
         <f t="shared" ref="D42:G42" si="40">D40*100^2/25^2</f>
@@ -4793,10 +4796,10 @@
     </row>
     <row r="43">
       <c r="B43" s="18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D43" s="15">
         <f t="shared" ref="D43:G43" si="43">ROUNDUP(SQRT(D39))</f>
@@ -4842,7 +4845,7 @@
     </row>
     <row r="44">
       <c r="C44" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D44" s="15">
         <f t="shared" ref="D44:G44" si="45">ROUNDUP(SQRT(D40))</f>
@@ -4888,7 +4891,7 @@
     </row>
     <row r="45">
       <c r="C45" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D45" s="15">
         <f t="shared" ref="D45:G45" si="48">ROUNDUP(SQRT(D41))</f>
@@ -4934,7 +4937,7 @@
     </row>
     <row r="46">
       <c r="C46" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D46" s="15">
         <f t="shared" ref="D46:G46" si="50">ROUNDUP(SQRT(D42))</f>
@@ -6182,16 +6185,20 @@
         <v>72</v>
       </c>
       <c r="B5" s="4">
-        <v>1.0</v>
+        <f t="shared" ref="B5:E5" si="1">B4/100/100</f>
+        <v>0.0025</v>
       </c>
       <c r="C5" s="4">
-        <v>3.0</v>
+        <f t="shared" si="1"/>
+        <v>0.005</v>
       </c>
       <c r="D5" s="4">
-        <v>2.0</v>
+        <f t="shared" si="1"/>
+        <v>0.005</v>
       </c>
       <c r="E5" s="4">
-        <v>10.0</v>
+        <f t="shared" si="1"/>
+        <v>0.01</v>
       </c>
     </row>
     <row r="6">
@@ -6199,16 +6206,16 @@
         <v>73</v>
       </c>
       <c r="B6" s="4">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C6" s="4">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="D6" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="E6" s="4">
         <v>10.0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>30.0</v>
       </c>
     </row>
     <row r="7">
@@ -6216,15 +6223,32 @@
         <v>74</v>
       </c>
       <c r="B7" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>30.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="4">
         <v>1.5</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C8" s="4">
         <v>3.0</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D8" s="4">
         <v>15.0</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E8" s="4">
         <v>45.0</v>
       </c>
     </row>
@@ -6246,26 +6270,26 @@
     <row r="1">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E2" s="3"/>
     </row>
@@ -6281,8 +6305,8 @@
         <v>600</v>
       </c>
       <c r="D3" s="12">
-        <f>C3*Economy!B4/Economy!B5/100</f>
-        <v>150</v>
+        <f>B3*Economy!B5/Economy!C6</f>
+        <v>0.375</v>
       </c>
     </row>
     <row r="4">
@@ -6297,8 +6321,8 @@
         <v>2000</v>
       </c>
       <c r="D4" s="15">
-        <f>C4*Economy!C4/Economy!C5/100</f>
-        <v>333.3333333</v>
+        <f>C4*Economy!C5/Economy!B6</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -6318,39 +6342,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3"/>
       <c r="B2" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B3" s="4">
         <v>-1.0</v>
@@ -6361,7 +6385,7 @@
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B4" s="4">
         <v>-1.0</v>
@@ -6372,7 +6396,7 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B5" s="4">
         <v>-1.0</v>
@@ -6383,7 +6407,7 @@
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B6" s="4">
         <v>-1.0</v>
@@ -6394,7 +6418,7 @@
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B7" s="4">
         <v>-1.0</v>
@@ -6405,7 +6429,7 @@
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B8" s="4">
         <v>-1.0</v>
@@ -6416,7 +6440,7 @@
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B9" s="4">
         <v>-1.0</v>
@@ -6427,7 +6451,7 @@
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B10" s="4">
         <v>-1.0</v>
@@ -6453,15 +6477,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B2" s="4">
         <v>80.0</v>
@@ -6469,7 +6493,7 @@
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B3" s="4">
         <v>5.0</v>
@@ -6477,7 +6501,7 @@
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B4" s="4">
         <v>5.0</v>
@@ -6485,7 +6509,7 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B5" s="4">
         <v>5.0</v>
@@ -6493,7 +6517,7 @@
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B6" s="4">
         <v>5.0</v>
@@ -6501,17 +6525,17 @@
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -6531,48 +6555,51 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
+      </c>
+      <c r="D2" s="4">
+        <v>-10.0</v>
       </c>
       <c r="G2" s="4">
         <v>-10.0</v>
@@ -6589,7 +6616,7 @@
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B3" s="4">
         <v>5.0</v>
@@ -6606,7 +6633,7 @@
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E4" s="4">
         <v>5.0</v>
@@ -6617,7 +6644,7 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E5" s="4">
         <v>-5.0</v>
@@ -6637,7 +6664,7 @@
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H6" s="4">
         <v>10.0</v>
@@ -6651,7 +6678,7 @@
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L7" s="4">
         <v>10.0</v>
@@ -6659,7 +6686,7 @@
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H8" s="4">
         <v>10.0</v>
@@ -6667,7 +6694,7 @@
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J9" s="4">
         <v>10.0</v>

</xml_diff>

<commit_message>
tune citizen food production
</commit_message>
<xml_diff>
--- a/Medieval Info.xlsx
+++ b/Medieval Info.xlsx
@@ -523,7 +523,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -562,6 +562,10 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -577,7 +581,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -618,6 +622,15 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="1" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -993,11 +1006,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="532613063"/>
-        <c:axId val="319222459"/>
+        <c:axId val="1751534799"/>
+        <c:axId val="1437237299"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="532613063"/>
+        <c:axId val="1751534799"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1049,10 +1062,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319222459"/>
+        <c:crossAx val="1437237299"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="319222459"/>
+        <c:axId val="1437237299"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1127,7 +1140,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="532613063"/>
+        <c:crossAx val="1751534799"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1219,11 +1232,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="422504406"/>
-        <c:axId val="567235271"/>
+        <c:axId val="1568007399"/>
+        <c:axId val="1397800739"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="422504406"/>
+        <c:axId val="1568007399"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1275,10 +1288,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="567235271"/>
+        <c:crossAx val="1397800739"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="567235271"/>
+        <c:axId val="1397800739"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1353,7 +1366,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422504406"/>
+        <c:crossAx val="1568007399"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1509,11 +1522,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="157024430"/>
-        <c:axId val="1984777209"/>
+        <c:axId val="329854027"/>
+        <c:axId val="92742886"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="157024430"/>
+        <c:axId val="329854027"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1565,10 +1578,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1984777209"/>
+        <c:crossAx val="92742886"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1984777209"/>
+        <c:axId val="92742886"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1643,7 +1656,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157024430"/>
+        <c:crossAx val="329854027"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1768,11 +1781,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1344402790"/>
-        <c:axId val="348381166"/>
+        <c:axId val="1236860477"/>
+        <c:axId val="928945772"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1344402790"/>
+        <c:axId val="1236860477"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1824,10 +1837,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348381166"/>
+        <c:crossAx val="928945772"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348381166"/>
+        <c:axId val="928945772"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1902,7 +1915,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1344402790"/>
+        <c:crossAx val="1236860477"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2027,11 +2040,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2130729286"/>
-        <c:axId val="1265249093"/>
+        <c:axId val="2000002570"/>
+        <c:axId val="1204525007"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2130729286"/>
+        <c:axId val="2000002570"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2083,10 +2096,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1265249093"/>
+        <c:crossAx val="1204525007"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1265249093"/>
+        <c:axId val="1204525007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2161,7 +2174,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130729286"/>
+        <c:crossAx val="2000002570"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3137,7 +3150,7 @@
       <c r="C1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="19" t="s">
         <v>123</v>
       </c>
       <c r="H1" s="3"/>
@@ -3163,7 +3176,7 @@
       <c r="C2" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="19" t="s">
         <v>126</v>
       </c>
       <c r="H2" s="3"/>
@@ -3188,7 +3201,7 @@
       <c r="C3" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="19" t="s">
         <v>130</v>
       </c>
       <c r="H3" s="3"/>
@@ -3213,7 +3226,7 @@
       <c r="C4" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="19" t="s">
         <v>134</v>
       </c>
       <c r="H4" s="3"/>
@@ -3799,7 +3812,7 @@
       </c>
       <c r="D21" s="12">
         <f>SUMPRODUCT(D11:D18,Citizens!$D$3:$D$10)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E21" s="12">
         <f>SUMPRODUCT(E11:E18,Citizens!$D$3:$D$10)</f>
@@ -3815,15 +3828,15 @@
       </c>
       <c r="I21" s="12">
         <f>SUMPRODUCT(I11:I18,Citizens!$D$3:$D$10)</f>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N21" s="12">
         <f>SUMPRODUCT(N11:N18,Citizens!$D$3:$D$10)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O21" s="12">
         <f>SUMPRODUCT(O11:O18,Citizens!$D$3:$D$10)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="P21" s="12">
         <f>SUMPRODUCT(P11:P18,Citizens!$D$3:$D$10)</f>
@@ -3831,7 +3844,7 @@
       </c>
       <c r="Q21" s="12">
         <f>SUMPRODUCT(Q11:Q18,Citizens!$D$3:$D$10)</f>
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="22">
@@ -3840,15 +3853,15 @@
       </c>
       <c r="D22" s="12">
         <f>SUMPRODUCT(D11:D18,Citizens!$E$3:$E$10)</f>
-        <v>5</v>
+        <v>3.75</v>
       </c>
       <c r="E22" s="12">
         <f>SUMPRODUCT(E11:E18,Citizens!$E$3:$E$10)</f>
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="F22" s="12">
         <f>SUMPRODUCT(F11:F18,Citizens!$E$3:$E$10)</f>
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="G22" s="12">
         <f>SUMPRODUCT(G11:G18,Citizens!$E$3:$E$10)</f>
@@ -3856,23 +3869,23 @@
       </c>
       <c r="I22" s="12">
         <f>SUMPRODUCT(I11:I18,Citizens!$E$3:$E$10)</f>
-        <v>30</v>
+        <v>22.5</v>
       </c>
       <c r="N22" s="12">
         <f>SUMPRODUCT(N11:N18,Citizens!$E$3:$E$10)</f>
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="O22" s="12">
         <f>SUMPRODUCT(O11:O18,Citizens!$E$3:$E$10)</f>
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="P22" s="12">
         <f>SUMPRODUCT(P11:P18,Citizens!$E$3:$E$10)</f>
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="Q22" s="12">
         <f>SUMPRODUCT(Q11:Q18,Citizens!$E$3:$E$10)</f>
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="23">
@@ -3887,7 +3900,7 @@
       </c>
       <c r="D23" s="12">
         <f t="shared" ref="D23:G23" si="5">D21+D19</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="E23" s="12">
         <f t="shared" si="5"/>
@@ -3903,15 +3916,15 @@
       </c>
       <c r="I23" s="12">
         <f t="shared" ref="I23:I24" si="8">I21+I19</f>
-        <v>-23</v>
+        <v>-20</v>
       </c>
       <c r="N23" s="12">
         <f t="shared" ref="N23:Q23" si="6">N21+N19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O23" s="12">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P23" s="12">
         <f t="shared" si="6"/>
@@ -3919,7 +3932,7 @@
       </c>
       <c r="Q23" s="12">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="24">
@@ -3928,15 +3941,15 @@
       </c>
       <c r="D24" s="12">
         <f t="shared" ref="D24:G24" si="7">D22+D20</f>
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="E24" s="12">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1.25</v>
       </c>
       <c r="F24" s="12">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1.25</v>
       </c>
       <c r="G24" s="12">
         <f t="shared" si="7"/>
@@ -3944,23 +3957,23 @@
       </c>
       <c r="I24" s="12">
         <f t="shared" si="8"/>
-        <v>19</v>
+        <v>11.5</v>
       </c>
       <c r="N24" s="12">
         <f t="shared" ref="N24:Q24" si="9">N22+N20</f>
-        <v>2</v>
+        <v>1.25</v>
       </c>
       <c r="O24" s="12">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1.25</v>
       </c>
       <c r="P24" s="12">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1.25</v>
       </c>
       <c r="Q24" s="12">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="25">
@@ -4216,10 +4229,10 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="21" t="s">
         <v>157</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -4412,7 +4425,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="21" t="s">
         <v>162</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -4599,10 +4612,10 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="21" t="s">
         <v>157</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -4795,7 +4808,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="21" t="s">
         <v>162</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -6278,7 +6291,6 @@
       <c r="D1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="2"/>
@@ -6291,7 +6303,6 @@
       <c r="D2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
@@ -6379,9 +6390,10 @@
       <c r="B3" s="4">
         <v>-1.0</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="16">
         <v>2.0</v>
       </c>
+      <c r="E3" s="17"/>
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
@@ -6390,9 +6402,10 @@
       <c r="B4" s="4">
         <v>-1.0</v>
       </c>
-      <c r="D4" s="4">
-        <v>2.0</v>
-      </c>
+      <c r="D4" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="E4" s="17"/>
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
@@ -6401,9 +6414,10 @@
       <c r="B5" s="4">
         <v>-1.0</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="16">
         <v>1.5</v>
       </c>
+      <c r="E5" s="17"/>
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
@@ -6412,8 +6426,9 @@
       <c r="B6" s="4">
         <v>-1.0</v>
       </c>
-      <c r="E6" s="4">
-        <v>1.0</v>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18">
+        <v>0.75</v>
       </c>
     </row>
     <row r="7">
@@ -6423,8 +6438,9 @@
       <c r="B7" s="4">
         <v>-1.0</v>
       </c>
-      <c r="E7" s="4">
-        <v>2.0</v>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18">
+        <v>1.5</v>
       </c>
     </row>
     <row r="8">

</xml_diff>